<commit_message>
add RelationalDatabaseTests for iot test/prod,add RestfulAsDataSourcesTests for iot dev
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B602BA0E-C14B-46EA-87D5-421C02ADB7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209DCF32-94F0-4D61-B88A-E21031E32651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3377,8 +3377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D398F-A510-45E2-94C1-EA62EAF2A2C6}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add api-engine new cases for sdl-5374
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209DCF32-94F0-4D61-B88A-E21031E32651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8834F3-BB5B-4290-A3B9-3E5D9D8E5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="250">
   <si>
     <t>description</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>[SensorData][type,Siid][{Siid: {_nin: [5040, 5045, 34155]}}][][]</t>
-  </si>
-  <si>
-    <t>{Plant {address id latitude longitude name plant_owner}}</t>
   </si>
   <si>
     <t>{Plan12321t {address id latitude longitude name plant_owner}}</t>
@@ -2404,6 +2401,50 @@
           operator: "Jeff Bezos"
         }</t>
   </si>
+  <si>
+    <t>iot-api-engine-graphql-test-12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request, data retrieved</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回数据条数即records，条数小于metadata里限定的100000条，可以正常得到数据</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-api-engine-graphql-test-13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bad request</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Plant {address id latitude longitude name plant_owner}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{SINAMICS_300_Log {update_time}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>exception: The number of reply records is greater than the max records</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回数据条数即records，条数大于metadata里限定的100001条，抛出异常</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{SINAMICS_300_Log(cond:"{Abs_actual_current_smoothed: {_gt: 199.999}}")  {update_time}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2413,33 +2454,33 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2813,7 +2854,7 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1"/>
@@ -2821,7 +2862,7 @@
     <col min="5" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2847,7 +2888,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2871,7 +2912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2895,7 +2936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2919,7 +2960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2943,7 +2984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2967,7 +3008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2991,7 +3032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -3015,7 +3056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3039,7 +3080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3072,25 +3113,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.21875" style="5" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="70.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -3110,18 +3151,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>245</v>
       </c>
       <c r="D2" s="6">
         <v>200</v>
@@ -3133,18 +3174,18 @@
         <v>10</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6">
         <v>200</v>
@@ -3153,21 +3194,21 @@
         <v>101301</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="6">
         <v>200</v>
@@ -3179,18 +3220,18 @@
         <v>10</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="6">
         <v>200</v>
@@ -3202,18 +3243,18 @@
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="6">
         <v>200</v>
@@ -3225,18 +3266,18 @@
         <v>29</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="6">
         <v>200</v>
@@ -3248,18 +3289,18 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="6">
         <v>200</v>
@@ -3271,18 +3312,18 @@
         <v>10</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="6">
         <v>200</v>
@@ -3291,21 +3332,21 @@
         <v>101301</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="6">
         <v>200</v>
@@ -3314,21 +3355,21 @@
         <v>101403</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6">
         <v>200</v>
@@ -3340,18 +3381,18 @@
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="6">
         <v>200</v>
@@ -3360,10 +3401,56 @@
         <v>100000</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>10</v>
+        <v>241</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" s="5">
+        <v>200</v>
+      </c>
+      <c r="E13" s="5">
+        <v>100000</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="5">
+        <v>200</v>
+      </c>
+      <c r="E14" s="5">
+        <v>101403</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3377,11 +3464,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D398F-A510-45E2-94C1-EA62EAF2A2C6}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="9" bestFit="1" customWidth="1"/>
@@ -3397,7 +3484,7 @@
     <col min="13" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -3405,19 +3492,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
@@ -3429,31 +3516,31 @@
         <v>4</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="G2" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="11">
         <v>200</v>
@@ -3468,28 +3555,28 @@
         <v>0</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="G3" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H3" s="11">
         <v>200</v>
@@ -3504,25 +3591,25 @@
         <v>0</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11">
@@ -3538,25 +3625,25 @@
         <v>1</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11">
@@ -3566,27 +3653,27 @@
         <v>101301</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11">
@@ -3596,27 +3683,27 @@
         <v>101301</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11">
@@ -3626,27 +3713,27 @@
         <v>101301</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11">
@@ -3656,32 +3743,32 @@
         <v>101301</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="H9" s="11">
         <v>200</v>
@@ -3696,30 +3783,30 @@
         <v>0</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="H10" s="11">
         <v>200</v>
@@ -3734,25 +3821,25 @@
         <v>0</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11">
@@ -3762,27 +3849,27 @@
         <v>101303</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11">
@@ -3792,27 +3879,27 @@
         <v>101301</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11">
@@ -3822,27 +3909,27 @@
         <v>101301</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11">
@@ -3852,27 +3939,27 @@
         <v>101301</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11">
@@ -3882,27 +3969,27 @@
         <v>101301</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11">
@@ -3918,30 +4005,30 @@
         <v>0</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H17" s="11">
         <v>200</v>
@@ -3956,30 +4043,30 @@
         <v>0</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="E18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H18" s="11">
         <v>200</v>
@@ -3994,30 +4081,30 @@
         <v>0</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="H19" s="11">
         <v>200</v>
@@ -4032,30 +4119,30 @@
         <v>0</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>166</v>
       </c>
       <c r="H20" s="11">
         <v>200</v>
@@ -4070,30 +4157,30 @@
         <v>0</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="H21" s="11">
         <v>200</v>
@@ -4108,30 +4195,30 @@
         <v>0</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>181</v>
-      </c>
       <c r="C22" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H22" s="11">
         <v>200</v>
@@ -4146,30 +4233,30 @@
         <v>0</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="C23" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H23" s="11">
         <v>200</v>
@@ -4184,30 +4271,30 @@
         <v>0</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="C24" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H24" s="11">
         <v>200</v>
@@ -4222,30 +4309,30 @@
         <v>0</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="H25" s="11">
         <v>200</v>
@@ -4260,30 +4347,30 @@
         <v>0</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="H26" s="11">
         <v>200</v>
@@ -4298,30 +4385,30 @@
         <v>0</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>215</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>216</v>
       </c>
       <c r="H27" s="11">
         <v>200</v>
@@ -4336,30 +4423,30 @@
         <v>0</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="H28" s="11">
         <v>200</v>
@@ -4374,30 +4461,30 @@
         <v>0</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="H29" s="11">
         <v>200</v>
@@ -4412,30 +4499,30 @@
         <v>0</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="H30" s="11">
         <v>200</v>
@@ -4450,30 +4537,30 @@
         <v>0</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="H31" s="11">
         <v>200</v>
@@ -4488,30 +4575,30 @@
         <v>0</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="E32" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="H32" s="11">
         <v>200</v>
@@ -4526,30 +4613,30 @@
         <v>0</v>
       </c>
       <c r="L32" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="C33" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="E33" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="H33" s="11">
         <v>200</v>
@@ -4564,30 +4651,30 @@
         <v>0</v>
       </c>
       <c r="L33" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="E34" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H34" s="11">
         <v>200</v>
@@ -4602,30 +4689,30 @@
         <v>0</v>
       </c>
       <c r="L34" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>168</v>
-      </c>
       <c r="E35" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H35" s="11">
         <v>200</v>
@@ -4640,30 +4727,30 @@
         <v>0</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="C36" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>178</v>
-      </c>
       <c r="E36" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H36" s="11">
         <v>200</v>
@@ -4678,30 +4765,30 @@
         <v>0</v>
       </c>
       <c r="L36" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="C37" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>184</v>
-      </c>
       <c r="E37" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H37" s="11">
         <v>200</v>
@@ -4716,30 +4803,30 @@
         <v>0</v>
       </c>
       <c r="L37" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>188</v>
-      </c>
       <c r="C38" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H38" s="11">
         <v>200</v>
@@ -4754,30 +4841,30 @@
         <v>0</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="H39" s="11">
         <v>200</v>
@@ -4792,30 +4879,30 @@
         <v>0</v>
       </c>
       <c r="L39" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="11" t="s">
         <v>202</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H40" s="11">
         <v>200</v>
@@ -4830,30 +4917,30 @@
         <v>0</v>
       </c>
       <c r="L40" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="C41" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="11" t="s">
+      <c r="E41" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="H41" s="11">
         <v>200</v>
@@ -4868,30 +4955,30 @@
         <v>0</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>220</v>
-      </c>
       <c r="E42" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H42" s="11">
         <v>200</v>
@@ -4906,27 +4993,27 @@
         <v>0</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11">
@@ -4942,7 +5029,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add read/write operation for Restful API as data source
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -5,17 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-with-comment\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8834F3-BB5B-4290-A3B9-3E5D9D8E5E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59D7E6A-FFF5-4637-ACCB-14EF8C4CC4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
     <sheet name="getDataGraphQL" sheetId="3" r:id="rId2"/>
     <sheet name="postGraphForMysql" sheetId="9" r:id="rId3"/>
+    <sheet name="restfulTransactionSingleEntity" sheetId="10" r:id="rId4"/>
+    <sheet name="restfulTransactionMultiEntity" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="280">
   <si>
     <t>description</t>
   </si>
@@ -2445,6 +2447,164 @@
     <t>{SINAMICS_300_Log(cond:"{Abs_actual_current_smoothed: {_gt: 199.999}}")  {update_time}}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>iot-restful-singleentity-test-1</t>
+  </si>
+  <si>
+    <t>good request,single simple entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>tableOfH2</t>
+  </si>
+  <si>
+    <t>USER_BASIC_INFO,USER_PROFILE</t>
+  </si>
+  <si>
+    <t>rspCodeOfH2</t>
+  </si>
+  <si>
+    <t>rspDataOfH2</t>
+  </si>
+  <si>
+    <t>expectResultOfUSER_BASIC_INFO</t>
+  </si>
+  <si>
+    <t>expectResultOfUSER_PROFILE</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+  ID: 1,
+  NAME: "xiaoming",
+  AGE: 12
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-2</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-3</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-4</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-5</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-6</t>
+  </si>
+  <si>
+    <t>iot-restful-singleentity-test-7</t>
+  </si>
+  <si>
+    <t>good request,single simple entity,update,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>good request,single simple entity,delete,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Update(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming.update",
+          age: 12,
+          mail: "xiaoming.update@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+  ID: 1,
+  NAME: "xiaoming.update",
+  AGE: 12
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming.update@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Delete(input:
+    [
+        {
+          id: 1
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>bad request,single simple entity,insert,transaction control</t>
+  </si>
+  <si>
+    <t>bad request,single simple entity,update,transaction control</t>
+  </si>
+  <si>
+    <t>bad request,single simple entity,delete,transaction control</t>
+  </si>
+  <si>
+    <t>INSERT INTO USER_BASIC_INFO VALUES (1,12,'xiaoming');
+INSERT INTO USER_PROFILE VALUES (1,'xiaoming@siemens.com','15245654568','beijing.china')</t>
+  </si>
+  <si>
+    <t>INSERT INTO USER_BASIC_INFO VALUES (1,12,'xiaoming')</t>
+  </si>
 </sst>
 </file>
 
@@ -2454,33 +2614,33 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2854,7 +3014,7 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1"/>
@@ -2862,7 +3022,7 @@
     <col min="5" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2888,7 +3048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2912,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2936,7 +3096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2960,7 +3120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2984,7 +3144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -3008,7 +3168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -3032,7 +3192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -3056,7 +3216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3080,7 +3240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -3115,11 +3275,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
@@ -3131,7 +3291,7 @@
     <col min="8" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -3154,7 +3314,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>76</v>
       </c>
@@ -3177,7 +3337,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
@@ -3200,7 +3360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>78</v>
       </c>
@@ -3223,7 +3383,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>79</v>
       </c>
@@ -3246,7 +3406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>80</v>
       </c>
@@ -3269,7 +3429,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>81</v>
       </c>
@@ -3292,7 +3452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>82</v>
       </c>
@@ -3315,7 +3475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
@@ -3338,7 +3498,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>84</v>
       </c>
@@ -3361,7 +3521,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>85</v>
       </c>
@@ -3384,7 +3544,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>86</v>
       </c>
@@ -3407,7 +3567,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>239</v>
       </c>
@@ -3430,7 +3590,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>243</v>
       </c>
@@ -3465,10 +3625,10 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="9" bestFit="1" customWidth="1"/>
@@ -3484,7 +3644,7 @@
     <col min="13" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -3522,7 +3682,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>58</v>
       </c>
@@ -3558,7 +3718,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>61</v>
       </c>
@@ -3594,7 +3754,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -3628,7 +3788,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>65</v>
       </c>
@@ -3658,7 +3818,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>66</v>
       </c>
@@ -3688,7 +3848,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>67</v>
       </c>
@@ -3718,7 +3878,7 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -3748,7 +3908,7 @@
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>59</v>
       </c>
@@ -3786,7 +3946,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>62</v>
       </c>
@@ -3824,7 +3984,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>69</v>
       </c>
@@ -3854,7 +4014,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>70</v>
       </c>
@@ -3884,7 +4044,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>71</v>
       </c>
@@ -3914,7 +4074,7 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>72</v>
       </c>
@@ -3944,7 +4104,7 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>73</v>
       </c>
@@ -3974,7 +4134,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>74</v>
       </c>
@@ -4008,7 +4168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>115</v>
       </c>
@@ -4046,7 +4206,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>117</v>
       </c>
@@ -4084,7 +4244,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>158</v>
       </c>
@@ -4122,7 +4282,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>164</v>
       </c>
@@ -4160,7 +4320,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>172</v>
       </c>
@@ -4198,7 +4358,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>179</v>
       </c>
@@ -4236,7 +4396,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>184</v>
       </c>
@@ -4274,7 +4434,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>191</v>
       </c>
@@ -4312,7 +4472,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>196</v>
       </c>
@@ -4350,7 +4510,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>203</v>
       </c>
@@ -4388,7 +4548,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>211</v>
       </c>
@@ -4426,7 +4586,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>212</v>
       </c>
@@ -4464,7 +4624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>60</v>
       </c>
@@ -4502,7 +4662,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>63</v>
       </c>
@@ -4540,7 +4700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>75</v>
       </c>
@@ -4578,7 +4738,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>116</v>
       </c>
@@ -4616,7 +4776,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>154</v>
       </c>
@@ -4654,7 +4814,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>160</v>
       </c>
@@ -4692,7 +4852,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>166</v>
       </c>
@@ -4730,7 +4890,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>175</v>
       </c>
@@ -4768,7 +4928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>181</v>
       </c>
@@ -4806,7 +4966,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>186</v>
       </c>
@@ -4844,7 +5004,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>193</v>
       </c>
@@ -4882,7 +5042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>199</v>
       </c>
@@ -4920,7 +5080,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>207</v>
       </c>
@@ -4958,7 +5118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>216</v>
       </c>
@@ -4996,7 +5156,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>217</v>
       </c>
@@ -5037,4 +5197,339 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F6F477-271A-41FE-A290-09DC67B3D45A}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="27" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="11">
+        <v>200</v>
+      </c>
+      <c r="J2" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="12">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I3" s="11">
+        <v>200</v>
+      </c>
+      <c r="J3" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
+        <v>200</v>
+      </c>
+      <c r="J4" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <v>200</v>
+      </c>
+      <c r="J5" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11">
+        <v>200</v>
+      </c>
+      <c r="J6" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11">
+        <v>200</v>
+      </c>
+      <c r="J7" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11">
+        <v>200</v>
+      </c>
+      <c r="J8" s="11">
+        <v>100000</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE618FA-BAFF-4947-8A48-6BBC9A48AE70}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add restfulTransactionSingleEntity/restfulTransactionMultiEntity in iot-api-engine-test-data.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DF27D1-4611-4B40-B65A-DBAF346AE0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C41DA1-8E6A-497D-A1B5-E3CAB316D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="346">
   <si>
     <t>description</t>
   </si>
@@ -2665,6 +2665,601 @@
    LOCATION: "Shanghai",
    QUANTITY: "excellent",
    SALES_ORDER:"12345678"
+}</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-1</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-2</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-3</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-4</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-5</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-6</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-7</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-8</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-9</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-10</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-11</t>
+  </si>
+  <si>
+    <t>iot-restful-multientity-test-12</t>
+  </si>
+  <si>
+    <t>good request,multi simple entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        },
+		{
+          id: 2,
+          name: "jojo",
+          age: 11,
+          mail: "jojo@live.cn",
+          phone: "13898786758",
+          address: "hangzhou.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        },
+		{
+          id: 2,
+          name: "jojo",
+          age: 11,
+          mail: "jojo@live.cn",
+          phone: "13898786758",
+          address: "hangzhou.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>User,Person</t>
+  </si>
+  <si>
+    <t>tableOfUser</t>
+  </si>
+  <si>
+    <t>tableOfPerson</t>
+  </si>
+  <si>
+    <t>tableOfProduct</t>
+  </si>
+  <si>
+    <t>pre-executionOfUser</t>
+  </si>
+  <si>
+    <t>pre-executionOfPerson</t>
+  </si>
+  <si>
+    <t>pre-executionOfProduct</t>
+  </si>
+  <si>
+    <t>expectResultOfPERSON_BASIC_INFO</t>
+  </si>
+  <si>
+    <t>expectResultOfPRODUCT</t>
+  </si>
+  <si>
+    <t>expectResultOfPRODUCT_ORDER</t>
+  </si>
+  <si>
+    <t>PERSON_BASIC_INFO,PERSON_PROFILE</t>
+  </si>
+  <si>
+    <t>{
+  ID: 1,
+  NAME: "xiaoming",
+  AGE: 12
+}
+{
+  ID: 2,
+  NAME: "jojo",
+  AGE: 11
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   USER_ID: 2,
+   MAIL: "jojo@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}</t>
+  </si>
+  <si>
+    <t>expectResultOfPERSON_PROFILE</t>
+  </si>
+  <si>
+    <t>{
+   PERSON_ID: 1,
+   MAIL: "xiaoming@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   PERSON_ID: 2,
+   MAIL: "jojo@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}</t>
+  </si>
+  <si>
+    <t>good/bad request,multi simple entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>INSERT INTO PERSON_BASIC_INFO VALUES (1,12,'xiaoming')</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>bad request,multi simple entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>good request,multi simple entity,update,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>good/bad request,multi simple entity,update,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>bad request,multi simple entity,update,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Update(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming.update",
+          age: 12,
+          mail: "xiaoming.update@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        },
+		{
+          id: 2,
+          name: "jojo.update",
+          age: 11,
+          mail: "jojo.update@live.cn",
+          phone: "13898786758",
+          address: "hangzhou.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Update(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming.update",
+          age: 12,
+          mail: "xiaoming.update@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        },
+		{
+          id: 2,
+          name: "jojo.update",
+          age: 11,
+          mail: "jojo.update@live.cn",
+          phone: "13898786758",
+          address: "hangzhou.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+  ID: 1,
+  NAME: "xiaoming.update",
+  AGE: 12
+}
+{
+  ID: 2,
+  NAME: "jojo.update",
+  AGE: 11
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming.update@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   USER_ID: 2,
+   MAIL: "jojo.update@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}</t>
+  </si>
+  <si>
+    <t>{
+   PERSON_ID: 1,
+   MAIL: "xiaoming.update@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   PERSON_ID: 2,
+   MAIL: "jojo.update@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}</t>
+  </si>
+  <si>
+    <t>INSERT INTO USER_BASIC_INFO VALUES (1,12,'xiaoming');
+INSERT INTO USER_PROFILE VALUES (1,'xiaoming@siemens.com','15245654568','beijing.china');
+INSERT INTO USER_BASIC_INFO VALUES (2,11,'jojo');
+INSERT INTO USER_PROFILE VALUES (2,'jojo@live.cn','13898786758','hangzhou.china')</t>
+  </si>
+  <si>
+    <t>INSERT INTO PERSON_BASIC_INFO VALUES (1,12,'xiaoming');
+INSERT INTO PERSON_PROFILE VALUES (1,'xiaoming@siemens.com','15245654568','beijing.china');
+INSERT INTO PERSON_BASIC_INFO VALUES (2,11,'jojo');
+INSERT INTO PERSON_PROFILE VALUES (2,'jojo@live.cn','13898786758','hangzhou.china')</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Update(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming.update",
+          age: 12,
+          mail: "xiaoming.update@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Update(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming.update",
+          age: 12,
+          mail: "xiaoming.update@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>INSERT INTO USER_BASIC_INFO VALUES (1,12,'xiaoming');</t>
+  </si>
+  <si>
+    <t>good request,multi simple entity,delete,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>good/bad request,multi simple entity,delete,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>bad request,multi simple entity,delete,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Delete(input:
+    [
+        {
+          id: 1
+        },
+		{
+          id: 2
+        },
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Delete(input:
+    [
+        {
+          id: 1
+        },
+		{
+          id: 2
+        },
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Delete(input:
+    [
+        {
+          id: 1
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Person_Delete(input:
+    [
+        {
+          id: 1
+        }
+     ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>User,Product</t>
+  </si>
+  <si>
+    <t>good request,multi complex entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>good/bad request,multi complex entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>bad request,multi complex entity,insert,transaction control,data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        },
+		{
+          id: 2,
+          name: "jojo",
+          age: 11,
+          mail: "jojo@live.cn",
+          phone: "13898786758",
+          address: "hangzhou.china"
+        },
+		{
+          id: 3,
+          name: "dongdong",
+          age: 15,
+          mail: "dongdong@siemens.com",
+          phone: "18787679898",
+          address: "suzhou.china"
+        }
+     ]
+    )
+	{
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Product_Insert(input:
+	[
+        {
+          name: "socks",
+          product_no: "2021-01-01T00:00:00",
+          product_type: "ladies",
+          description: "cotton",
+          Product_Order:
+            {
+              product: "sports socks",
+              type: "Women's sports socks",
+              location: "Shanghai",
+              quantity: "excellent",
+              sales_order: "12345678"
+            }
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+  ID: 1,
+  NAME: "xiaoming",
+  AGE: 12
+}
+{
+  ID: 2,
+  NAME: "jojo",
+  AGE: 11
+}
+{
+  ID: 3,
+  NAME: "dongdong",
+  AGE: 15
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   USER_ID: 2,
+   MAIL: "jojo@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}
+   USER_ID: 3,
+   MAIL: "dongdong@siemens.com",
+   PHONE: "18787679898",
+   ADDRESS: "suzhou.china"
+}</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    User_Insert(input:
+    [
+        {
+          id: 1,
+          name: "xiaoming",
+          age: 12,
+          mail: "xiaoming@siemens.com",
+          phone: "15245654568",
+          address: "beijing.china"
+        }
+     ]
+    )
+	{
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+	Product_Insert(input:
+	[
+        {
+          name: "socks",
+          product_no: "2021-01-01T00:00:00",
+          product_type: "ladies",
+          description: "cotton",
+          Product_Order:
+            {
+              product: "sports socks",
+              type: "Women's sports socks",
+              location: "Shanghai",
+              quantity: "excellent",
+              sales_order: "12345678"
+            }
+        }
+    ]
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
 }</t>
   </si>
 </sst>
@@ -5265,8 +5860,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F6F477-271A-41FE-A290-09DC67B3D45A}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5624,14 +6220,659 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE618FA-BAFF-4947-8A48-6BBC9A48AE70}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="44.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="26.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11">
+        <v>200</v>
+      </c>
+      <c r="R2" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11">
+        <v>200</v>
+      </c>
+      <c r="R3" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11">
+        <v>200</v>
+      </c>
+      <c r="R4" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11">
+        <v>200</v>
+      </c>
+      <c r="R5" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11">
+        <v>200</v>
+      </c>
+      <c r="R6" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11">
+        <v>200</v>
+      </c>
+      <c r="R7" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11">
+        <v>200</v>
+      </c>
+      <c r="R8" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11">
+        <v>200</v>
+      </c>
+      <c r="R9" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11">
+        <v>200</v>
+      </c>
+      <c r="R10" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>200</v>
+      </c>
+      <c r="R11" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S11" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11">
+        <v>200</v>
+      </c>
+      <c r="R12" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11">
+        <v>200</v>
+      </c>
+      <c r="R13" s="11">
+        <v>100000</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
modify case of 'restful as data soure'
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C41DA1-8E6A-497D-A1B5-E3CAB316D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094C9E84-D605-4048-997F-6F5BE5F71301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="346">
   <si>
     <t>description</t>
   </si>
@@ -3200,25 +3200,6 @@
 }</t>
   </si>
   <si>
-    <t>{
-   USER_ID: 1,
-   MAIL: "xiaoming@siemens.com",
-   PHONE: "15245654568",
-   ADDRESS: "beijing.china"
-}
-{
-   USER_ID: 2,
-   MAIL: "jojo@live.cn",
-   PHONE: "13898786758",
-   ADDRESS: "hangzhou.china"
-}
-   USER_ID: 3,
-   MAIL: "dongdong@siemens.com",
-   PHONE: "18787679898",
-   ADDRESS: "suzhou.china"
-}</t>
-  </si>
-  <si>
     <t>mutation mutationName{
     User_Insert(input:
     [
@@ -3260,6 +3241,26 @@
         reserved_field_1
         reserved_field_2
     }
+}</t>
+  </si>
+  <si>
+    <t>{
+   USER_ID: 1,
+   MAIL: "xiaoming@siemens.com",
+   PHONE: "15245654568",
+   ADDRESS: "beijing.china"
+}
+{
+   USER_ID: 2,
+   MAIL: "jojo@live.cn",
+   PHONE: "13898786758",
+   ADDRESS: "hangzhou.china"
+}
+{
+   USER_ID: 3,
+   MAIL: "dongdong@siemens.com",
+   PHONE: "18787679898",
+   ADDRESS: "suzhou.china"
 }</t>
   </si>
 </sst>
@@ -3933,7 +3934,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4225,48 +4226,48 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D13" s="5">
-        <v>200</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="D13" s="6">
+        <v>200</v>
+      </c>
+      <c r="E13" s="6">
         <v>100000</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D14" s="5">
-        <v>200</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="D14" s="6">
+        <v>200</v>
+      </c>
+      <c r="E14" s="6">
         <v>101403</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4281,8 +4282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D398F-A510-45E2-94C1-EA62EAF2A2C6}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5858,11 +5859,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F6F477-271A-41FE-A290-09DC67B3D45A}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8:H8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5872,17 +5873,18 @@
     <col min="3" max="4" width="31.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="33.21875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="38.5546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="9"/>
+    <col min="7" max="7" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.21875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="38.5546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -5902,28 +5904,31 @@
         <v>254</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>250</v>
       </c>
@@ -5941,26 +5946,29 @@
         <v>255</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="I2" s="11">
-        <v>200</v>
-      </c>
       <c r="J2" s="11">
+        <v>200</v>
+      </c>
+      <c r="K2" s="11">
         <v>100000</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12">
+      <c r="M2" s="12">
         <v>0</v>
       </c>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>263</v>
       </c>
@@ -5980,26 +5988,29 @@
         <v>255</v>
       </c>
       <c r="G3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="I3" s="11">
-        <v>200</v>
-      </c>
       <c r="J3" s="11">
+        <v>200</v>
+      </c>
+      <c r="K3" s="11">
         <v>100000</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>264</v>
       </c>
@@ -6018,23 +6029,26 @@
       <c r="F4" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="11">
-        <v>200</v>
-      </c>
+      <c r="I4" s="11"/>
       <c r="J4" s="11">
+        <v>200</v>
+      </c>
+      <c r="K4" s="11">
         <v>100000</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="12">
+      <c r="M4" s="12">
         <v>0</v>
       </c>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>265</v>
       </c>
@@ -6054,24 +6068,27 @@
         <v>255</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11">
-        <v>200</v>
-      </c>
+      <c r="I5" s="11"/>
       <c r="J5" s="11">
+        <v>200</v>
+      </c>
+      <c r="K5" s="11">
         <v>100000</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="12">
+      <c r="M5" s="12">
         <v>0</v>
       </c>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>266</v>
       </c>
@@ -6091,24 +6108,27 @@
         <v>255</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11">
-        <v>200</v>
-      </c>
+      <c r="I6" s="11"/>
       <c r="J6" s="11">
+        <v>200</v>
+      </c>
+      <c r="K6" s="11">
         <v>100000</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="12">
+      <c r="M6" s="12">
         <v>0</v>
       </c>
-      <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>267</v>
       </c>
@@ -6128,24 +6148,27 @@
         <v>255</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11">
-        <v>200</v>
-      </c>
+      <c r="I7" s="11"/>
       <c r="J7" s="11">
+        <v>200</v>
+      </c>
+      <c r="K7" s="11">
         <v>100000</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="12">
+      <c r="M7" s="12">
         <v>0</v>
       </c>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="13"/>
+    </row>
+    <row r="8" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>268</v>
       </c>
@@ -6163,26 +6186,29 @@
         <v>285</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="I8" s="11">
-        <v>200</v>
-      </c>
       <c r="J8" s="11">
+        <v>200</v>
+      </c>
+      <c r="K8" s="11">
         <v>100000</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="12">
+      <c r="M8" s="12">
         <v>0</v>
       </c>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>281</v>
       </c>
@@ -6202,14 +6228,25 @@
         <v>285</v>
       </c>
       <c r="G9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13"/>
+      <c r="J9" s="11">
+        <v>200</v>
+      </c>
+      <c r="K9" s="11">
+        <v>100000</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
+      <c r="N9" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6223,8 +6260,8 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6757,7 +6794,7 @@
         <v>343</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -6793,7 +6830,7 @@
         <v>286</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>255</v>
@@ -6842,7 +6879,7 @@
         <v>286</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>255</v>

</xml_diff>

<commit_message>
add test cases of AuthForRestfulWriteTests
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4FF039-41B1-4B11-BE73-53095704DD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971CF752-8D58-496B-8459-A817E5939EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="postGraphForMysql" sheetId="9" r:id="rId3"/>
     <sheet name="restfulTransactionSingleEntity" sheetId="10" r:id="rId4"/>
     <sheet name="restfulTransactionMultiEntity" sheetId="11" r:id="rId5"/>
+    <sheet name="authForRestfulWrite" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="390">
   <si>
     <t>description</t>
   </si>
@@ -3262,6 +3263,399 @@
    PHONE: "18787679898",
    ADDRESS: "suzhou.china"
 }</t>
+  </si>
+  <si>
+    <t>good request,insert one entity of basic/oauth/cookie/token auth type success, data retrieved</t>
+  </si>
+  <si>
+    <t>authList</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    UserWithAuth_Insert(input:
+    [
+        {
+          id: 1,
+          name: "XiaoMing",
+          age: 26,
+          mail: "Ming.Xiao@siemens.com",
+          phone: "15245654568",
+          address: "Beijing.China",
+          employer:"Siemens",
+          title:"engineer",
+          employeeid:"A006WFRV",
+          mothertongue:"mandarin",
+          secondlanguage:"English",
+          course:"Advanced mathematics"
+        }
+    ],
+    authInfo:"$authInfo"
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserBasicInfoWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    },
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserProfileWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    },
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserWorkWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    },
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserSpecialtyWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>UserWithAuth</t>
+  </si>
+  <si>
+    <t>rspDataOfRestful</t>
+  </si>
+  <si>
+    <t>rspCodeOfRestful</t>
+  </si>
+  <si>
+    <t>bad request,insert one entity of
+basic auth type:fail
+oauth auth type:success
+cookie auth type:success
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,insert one entity of
+basic auth type:success
+oauth auth type:fail
+cookie auth type:success
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,insert one entity of
+basic auth type:success
+oauth auth type:success
+cookie auth type:fail
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,insert one entity of
+basic auth type:success
+oauth auth type:success
+cookie auth type:success
+token auth type:fail</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserBasicInfoWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123457"
+        }
+    },
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserProfileWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    },
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserWorkWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    },
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserSpecialtyWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserBasicInfoWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    },
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserProfileWithOauthAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    },
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserWorkWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    },
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserSpecialtyWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserBasicInfoWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    },
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserProfileWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    },
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserWorkWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value3"
+        }
+    },
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserSpecialtyWithTokenAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "authType":"basic",
+        "dataSourceName":"UserBasicInfoWithBasicAuth",
+        "detail":{
+            "value":"name=admin pwd=123456"
+        }
+    },
+    {
+        "authType":"OAUTH",
+        "dataSourceName":"UserProfileWithOauthAuth",
+        "detail":{
+            "value":"admin123456"
+        }
+    },
+    {
+        "authType":"Cookie",
+        "dataSourceName":"UserWorkWithCookieAuth",
+        "detail":{
+            "value":"key1=value1;key2=value2"
+        }
+    },
+    {
+        "authType":"TOKEN",
+        "dataSourceName":"UserSpecialtyWithTokenAuth",
+        "detail":{
+            "value":"admin123457"
+        }
+    }
+]</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-insert-test-1</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-insert-test-2</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-insert-test-3</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-insert-test-4</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-insert-test-5</t>
+  </si>
+  <si>
+    <t>{
+   UserBasicInfoWithBasicAuth:200,
+   UserProfileWithOauthAuth:200,
+   UserWorkWithCookieAuth:200,   UserSpecialtyWithTokenAuth:200
+}</t>
+  </si>
+  <si>
+    <t>{
+   UserBasicInfoWithBasicAuth:200,
+   UserProfileWithOauthAuth:401,
+   UserWorkWithCookieAuth:200,   UserSpecialtyWithTokenAuth:200
+}</t>
+  </si>
+  <si>
+    <t>{
+   UserBasicInfoWithBasicAuth:401,
+   UserProfileWithOauthAuth:200,
+   UserWorkWithCookieAuth:200,   UserSpecialtyWithTokenAuth:200
+}</t>
+  </si>
+  <si>
+    <t>{
+   UserBasicInfoWithBasicAuth:200,
+   UserProfileWithOauthAuth:200,
+   UserWorkWithCookieAuth:401,   UserSpecialtyWithTokenAuth:200
+}</t>
+  </si>
+  <si>
+    <t>{
+   UserBasicInfoWithBasicAuth:200,
+   UserProfileWithOauthAuth:200,
+   UserWorkWithCookieAuth:200,   UserSpecialtyWithTokenAuth:401
+}</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-update-test-1</t>
+  </si>
+  <si>
+    <t>good request,updatet one entity of basic/oauth/cookie/token auth type success, data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    UserWithAuth_Update(input:
+    [
+        {
+          id: 1,
+          name: "XiaoMing.Update",
+          age: 26,
+          mail: "Ming.Xiao.Update@siemens.com",
+          phone: "15245654568",
+          address: "Beijing.China",
+          employer:"Siemens",
+          title:"engineer",
+          employeeid:"A006WFRV",
+          mothertongue:"mandarin",
+          secondlanguage:"English",
+          course:"Advanced mathematics"
+        }
+    ],
+    authInfo:"$authInfo"
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-update-test-2</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-update-test-3</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-update-test-4</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-update-test-5</t>
+  </si>
+  <si>
+    <t>bad request,update one entity of
+basic auth type:fail
+oauth auth type:success
+cookie auth type:success
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,update one entity of
+basic auth type:success
+oauth auth type:fail
+cookie auth type:success
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,update one entity of
+basic auth type:success
+oauth auth type:success
+cookie auth type:fail
+token auth type:success</t>
+  </si>
+  <si>
+    <t>bad request,update one entity of
+basic auth type:success
+oauth auth type:success
+cookie auth type:success
+token auth type:fail</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-delete-test-1</t>
+  </si>
+  <si>
+    <t>good request,delete one entity of basic/oauth/cookie/token auth type success, data retrieved</t>
+  </si>
+  <si>
+    <t>mutation mutationName{
+    UserWithAuth_Delete(input:
+    [
+        {
+          id: 1
+        }
+    ],
+    authInfo:"$authInfo"
+    )
+    {
+        json_value
+        reserved_field_1
+        reserved_field_2
+    }
+}</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-delete-test-2</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-delete-test-3</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-delete-test-4</t>
+  </si>
+  <si>
+    <t>iot-restful-write-auth-delete-test-5</t>
   </si>
 </sst>
 </file>
@@ -4282,8 +4676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D398F-A510-45E2-94C1-EA62EAF2A2C6}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5861,9 +6255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F6F477-271A-41FE-A290-09DC67B3D45A}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6284,8 +6678,8 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6940,4 +7334,595 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD7C303-AF77-4B95-95EB-BAA32E85C8DA}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="38.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="38.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="11">
+        <v>200</v>
+      </c>
+      <c r="H2" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="11">
+        <v>200</v>
+      </c>
+      <c r="H3" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="12">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="11">
+        <v>200</v>
+      </c>
+      <c r="H4" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="11">
+        <v>200</v>
+      </c>
+      <c r="H5" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="11">
+        <v>200</v>
+      </c>
+      <c r="H6" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="11">
+        <v>200</v>
+      </c>
+      <c r="H7" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="11">
+        <v>200</v>
+      </c>
+      <c r="H8" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="11">
+        <v>200</v>
+      </c>
+      <c r="H9" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="11">
+        <v>200</v>
+      </c>
+      <c r="H10" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="11">
+        <v>200</v>
+      </c>
+      <c r="H11" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="12">
+        <v>1</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="11">
+        <v>200</v>
+      </c>
+      <c r="H12" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="11">
+        <v>200</v>
+      </c>
+      <c r="H13" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="11">
+        <v>200</v>
+      </c>
+      <c r="H14" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="11">
+        <v>200</v>
+      </c>
+      <c r="H15" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="11">
+        <v>200</v>
+      </c>
+      <c r="H16" s="11">
+        <v>100000</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify test case of mysql:delete code of connect to mysql
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971CF752-8D58-496B-8459-A817E5939EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE49385E-E135-489B-A116-CE16873AFAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
     <sheet name="getDataGraphQL" sheetId="3" r:id="rId2"/>
-    <sheet name="postGraphForMysql" sheetId="9" r:id="rId3"/>
-    <sheet name="restfulTransactionSingleEntity" sheetId="10" r:id="rId4"/>
-    <sheet name="restfulTransactionMultiEntity" sheetId="11" r:id="rId5"/>
-    <sheet name="authForRestfulWrite" sheetId="12" r:id="rId6"/>
+    <sheet name="postGraphForMysql" sheetId="14" r:id="rId3"/>
+    <sheet name="postGraphForMysql-backup" sheetId="9" r:id="rId4"/>
+    <sheet name="restfulTransactionSingleEntity" sheetId="10" r:id="rId5"/>
+    <sheet name="restfulTransactionMultiEntity" sheetId="11" r:id="rId6"/>
+    <sheet name="authForRestfulWrite" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="400">
   <si>
     <t>description</t>
   </si>
@@ -3656,6 +3657,36 @@
   </si>
   <si>
     <t>iot-restful-write-auth-delete-test-5</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6</t>
+  </si>
+  <si>
+    <t>expectedRemainingIdInMysql</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>1,4,5,6</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>1,5,6</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>1,2,3,4,6</t>
   </si>
 </sst>
 </file>
@@ -4673,11 +4704,1591 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DC2BAC-5C19-4CFF-8624-044FD1CB4C77}">
+  <dimension ref="A1:L43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>200</v>
+      </c>
+      <c r="I2" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H3" s="11">
+        <v>200</v>
+      </c>
+      <c r="I3" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11">
+        <v>200</v>
+      </c>
+      <c r="I4" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11">
+        <v>200</v>
+      </c>
+      <c r="I5" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11">
+        <v>200</v>
+      </c>
+      <c r="I6" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11">
+        <v>200</v>
+      </c>
+      <c r="I7" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11">
+        <v>200</v>
+      </c>
+      <c r="I8" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11">
+        <v>200</v>
+      </c>
+      <c r="I9" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H10" s="11">
+        <v>200</v>
+      </c>
+      <c r="I10" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11">
+        <v>200</v>
+      </c>
+      <c r="I11" s="11">
+        <v>101303</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11">
+        <v>200</v>
+      </c>
+      <c r="I12" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11">
+        <v>200</v>
+      </c>
+      <c r="I13" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11">
+        <v>200</v>
+      </c>
+      <c r="I14" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11">
+        <v>200</v>
+      </c>
+      <c r="I15" s="11">
+        <v>101301</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11">
+        <v>200</v>
+      </c>
+      <c r="I16" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H17" s="11">
+        <v>200</v>
+      </c>
+      <c r="I17" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H18" s="11">
+        <v>200</v>
+      </c>
+      <c r="I18" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H19" s="11">
+        <v>200</v>
+      </c>
+      <c r="I19" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H20" s="11">
+        <v>200</v>
+      </c>
+      <c r="I20" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H21" s="11">
+        <v>200</v>
+      </c>
+      <c r="I21" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H22" s="11">
+        <v>200</v>
+      </c>
+      <c r="I22" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="11">
+        <v>0</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H23" s="11">
+        <v>200</v>
+      </c>
+      <c r="I23" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H24" s="11">
+        <v>200</v>
+      </c>
+      <c r="I24" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H25" s="11">
+        <v>200</v>
+      </c>
+      <c r="I25" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H26" s="11">
+        <v>200</v>
+      </c>
+      <c r="I26" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H27" s="11">
+        <v>200</v>
+      </c>
+      <c r="I27" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H28" s="11">
+        <v>200</v>
+      </c>
+      <c r="I28" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="11">
+        <v>0</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H29" s="11">
+        <v>200</v>
+      </c>
+      <c r="I29" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="11">
+        <v>0</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="H30" s="11">
+        <v>200</v>
+      </c>
+      <c r="I30" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="H31" s="11">
+        <v>200</v>
+      </c>
+      <c r="I31" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="11">
+        <v>0</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="H32" s="11">
+        <v>200</v>
+      </c>
+      <c r="I32" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="11">
+        <v>0</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1</v>
+      </c>
+      <c r="H33" s="11">
+        <v>200</v>
+      </c>
+      <c r="I33" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="11">
+        <v>0</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="H34" s="11">
+        <v>200</v>
+      </c>
+      <c r="I34" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="11">
+        <v>0</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="H35" s="11">
+        <v>200</v>
+      </c>
+      <c r="I35" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="11">
+        <v>0</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H36" s="11">
+        <v>200</v>
+      </c>
+      <c r="I36" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="11">
+        <v>0</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="H37" s="11">
+        <v>200</v>
+      </c>
+      <c r="I37" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="11">
+        <v>0</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="11">
+        <v>6</v>
+      </c>
+      <c r="H38" s="11">
+        <v>200</v>
+      </c>
+      <c r="I38" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="H39" s="11">
+        <v>200</v>
+      </c>
+      <c r="I39" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="11">
+        <v>0</v>
+      </c>
+      <c r="L39" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="H40" s="11">
+        <v>200</v>
+      </c>
+      <c r="I40" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="11">
+        <v>0</v>
+      </c>
+      <c r="L40" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="H41" s="11">
+        <v>200</v>
+      </c>
+      <c r="I41" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="11">
+        <v>0</v>
+      </c>
+      <c r="L41" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="H42" s="11">
+        <v>200</v>
+      </c>
+      <c r="I42" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="11">
+        <v>0</v>
+      </c>
+      <c r="L42" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="10" customFormat="1" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11">
+        <v>200</v>
+      </c>
+      <c r="I43" s="11">
+        <v>100000</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="11">
+        <v>0</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D398F-A510-45E2-94C1-EA62EAF2A2C6}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6251,12 +7862,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F6F477-271A-41FE-A290-09DC67B3D45A}">
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -6673,7 +8284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE618FA-BAFF-4947-8A48-6BBC9A48AE70}">
   <dimension ref="A1:S13"/>
   <sheetViews>
@@ -7336,11 +8947,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD7C303-AF77-4B95-95EB-BAA32E85C8DA}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add test cases for SDL-8011
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4826E559-C532-4ABE-A937-1494BF853726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBEE927-D534-425B-A3B7-808922276F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="857">
   <si>
     <t>description</t>
   </si>
@@ -7451,6 +7451,12 @@
       "reserved_field_2": null
     }
   }</t>
+  </si>
+  <si>
+    <t>good request,
+delete operation,
+By Condition,
+3 data retrieved</t>
   </si>
 </sst>
 </file>
@@ -8471,9 +8477,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DC2BAC-5C19-4CFF-8624-044FD1CB4C77}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -8625,17 +8631,13 @@
         <v>200</v>
       </c>
       <c r="I4" s="11">
-        <v>100000</v>
+        <v>101403</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="11">
-        <v>1</v>
-      </c>
-      <c r="L4" s="11" t="s">
         <v>109</v>
       </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
@@ -8719,17 +8721,13 @@
         <v>200</v>
       </c>
       <c r="I7" s="11">
-        <v>100000</v>
+        <v>101403</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="11">
-        <v>1</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>399</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
@@ -9203,17 +9201,13 @@
         <v>200</v>
       </c>
       <c r="I21" s="11">
-        <v>100000</v>
+        <v>101403</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="11">
-        <v>0</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>102</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
     </row>
     <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
@@ -13314,8 +13308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD7D6DE-617D-4A49-9D87-297640E0E1DC}">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -16428,7 +16422,7 @@
         <v>585</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>512</v>
+        <v>578</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>682</v>
@@ -16454,7 +16448,7 @@
         <v>586</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>521</v>
+        <v>856</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>682</v>
@@ -16480,7 +16474,7 @@
         <v>587</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>523</v>
+        <v>607</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>682</v>
@@ -16662,7 +16656,7 @@
         <v>595</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>512</v>
+        <v>578</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>738</v>
@@ -16688,7 +16682,7 @@
         <v>596</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>521</v>
+        <v>856</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>738</v>
@@ -16714,7 +16708,7 @@
         <v>597</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>523</v>
+        <v>607</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>738</v>
@@ -16896,7 +16890,7 @@
         <v>604</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>512</v>
+        <v>578</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>778</v>
@@ -16922,7 +16916,7 @@
         <v>605</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>521</v>
+        <v>856</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>778</v>

</xml_diff>

<commit_message>
Modify the description of Epic / feature / story / test description
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBEE927-D534-425B-A3B7-808922276F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F05BDA-765E-49F6-95DE-70B694A277C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -8478,8 +8478,8 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21:L21"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -8724,7 +8724,7 @@
         <v>101403</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>109</v>
+        <v>399</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -8947,17 +8947,13 @@
         <v>200</v>
       </c>
       <c r="I14" s="11">
-        <v>100000</v>
+        <v>101403</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="11">
-        <v>1</v>
-      </c>
-      <c r="L14" s="11" t="s">
         <v>399</v>
       </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
@@ -9201,13 +9197,17 @@
         <v>200</v>
       </c>
       <c r="I21" s="11">
-        <v>101403</v>
+        <v>100000</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="K21" s="11">
+        <v>0</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">

</xml_diff>

<commit_message>
Modify the way to test SQL Server
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA79F0F0-263D-4B8B-B468-16DAE67159AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2096CF-CA9A-48DC-9451-CEE98219F488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="readWriteMySQL" sheetId="22" r:id="rId4"/>
     <sheet name="readPostgreSQL" sheetId="18" r:id="rId5"/>
     <sheet name="writePostgreSQL" sheetId="17" r:id="rId6"/>
-    <sheet name="readWriteSqlServer" sheetId="23" r:id="rId7"/>
+    <sheet name="readWriteSqlServer" sheetId="25" r:id="rId7"/>
     <sheet name="readWriteH2" sheetId="24" r:id="rId8"/>
     <sheet name="restfulTransactionSingleEntity" sheetId="10" r:id="rId9"/>
     <sheet name="restfulTransactionMultiEntity" sheetId="11" r:id="rId10"/>
@@ -27,6 +27,7 @@
     <sheet name="transferOfFlexibleParams" sheetId="16" r:id="rId12"/>
     <sheet name="testWhichVerifyRspdata" sheetId="19" r:id="rId13"/>
     <sheet name="testMultiDataSource" sheetId="20" r:id="rId14"/>
+    <sheet name="readWriteSqlServer-bc" sheetId="23" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3401" uniqueCount="1574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="1575">
   <si>
     <t>description</t>
   </si>
@@ -16644,6 +16645,9 @@
         }
     ]
 }</t>
+  </si>
+  <si>
+    <t>SqlServer_Test</t>
   </si>
 </sst>
 </file>
@@ -22674,6 +22678,1740 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A66780-5999-4CB7-B600-95BB7A39B0F9}">
+  <dimension ref="A1:J56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F2" s="4">
+        <v>200</v>
+      </c>
+      <c r="G2" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F3" s="4">
+        <v>200</v>
+      </c>
+      <c r="G3" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1280</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F4" s="4">
+        <v>200</v>
+      </c>
+      <c r="G4" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F6" s="4">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F7" s="4">
+        <v>200</v>
+      </c>
+      <c r="G7" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>1280</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F8" s="4">
+        <v>200</v>
+      </c>
+      <c r="G8" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F9" s="4">
+        <v>200</v>
+      </c>
+      <c r="G9" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>1296</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F10" s="4">
+        <v>200</v>
+      </c>
+      <c r="G10" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>1299</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F11" s="4">
+        <v>200</v>
+      </c>
+      <c r="G11" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>1280</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F12" s="4">
+        <v>200</v>
+      </c>
+      <c r="G12" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>1304</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F13" s="4">
+        <v>200</v>
+      </c>
+      <c r="G13" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F14" s="4">
+        <v>200</v>
+      </c>
+      <c r="G14" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>1277</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F15" s="4">
+        <v>200</v>
+      </c>
+      <c r="G15" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>1312</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F16" s="4">
+        <v>200</v>
+      </c>
+      <c r="G16" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F17" s="4">
+        <v>200</v>
+      </c>
+      <c r="G17" s="4">
+        <v>101403</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>983</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F18" s="4">
+        <v>200</v>
+      </c>
+      <c r="G18" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F19" s="4">
+        <v>200</v>
+      </c>
+      <c r="G19" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F20" s="7">
+        <v>200</v>
+      </c>
+      <c r="G20" s="7">
+        <v>101403</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F21" s="4">
+        <v>200</v>
+      </c>
+      <c r="G21" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F22" s="4">
+        <v>200</v>
+      </c>
+      <c r="G22" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F23" s="4">
+        <v>200</v>
+      </c>
+      <c r="G23" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F24" s="4">
+        <v>200</v>
+      </c>
+      <c r="G24" s="4">
+        <v>101303</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F25" s="4">
+        <v>200</v>
+      </c>
+      <c r="G25" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F26" s="4">
+        <v>200</v>
+      </c>
+      <c r="G26" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F27" s="7">
+        <v>200</v>
+      </c>
+      <c r="G27" s="7">
+        <v>101403</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F28" s="4">
+        <v>200</v>
+      </c>
+      <c r="G28" s="4">
+        <v>101301</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F29" s="4">
+        <v>200</v>
+      </c>
+      <c r="G29" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F30" s="4">
+        <v>200</v>
+      </c>
+      <c r="G30" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F31" s="4">
+        <v>200</v>
+      </c>
+      <c r="G31" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F32" s="4">
+        <v>200</v>
+      </c>
+      <c r="G32" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F33" s="4">
+        <v>200</v>
+      </c>
+      <c r="G33" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F34" s="4">
+        <v>200</v>
+      </c>
+      <c r="G34" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F35" s="4">
+        <v>200</v>
+      </c>
+      <c r="G35" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F36" s="4">
+        <v>200</v>
+      </c>
+      <c r="G36" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F37" s="4">
+        <v>200</v>
+      </c>
+      <c r="G37" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F38" s="4">
+        <v>200</v>
+      </c>
+      <c r="G38" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F39" s="4">
+        <v>200</v>
+      </c>
+      <c r="G39" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F40" s="4">
+        <v>200</v>
+      </c>
+      <c r="G40" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F41" s="4">
+        <v>200</v>
+      </c>
+      <c r="G41" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F42" s="4">
+        <v>200</v>
+      </c>
+      <c r="G42" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F43" s="4">
+        <v>200</v>
+      </c>
+      <c r="G43" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F44" s="4">
+        <v>200</v>
+      </c>
+      <c r="G44" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F45" s="4">
+        <v>200</v>
+      </c>
+      <c r="G45" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F46" s="4">
+        <v>200</v>
+      </c>
+      <c r="G46" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F47" s="4">
+        <v>200</v>
+      </c>
+      <c r="G47" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F48" s="4">
+        <v>200</v>
+      </c>
+      <c r="G48" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F49" s="4">
+        <v>200</v>
+      </c>
+      <c r="G49" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F50" s="4">
+        <v>200</v>
+      </c>
+      <c r="G50" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F51" s="4">
+        <v>200</v>
+      </c>
+      <c r="G51" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F52" s="4">
+        <v>200</v>
+      </c>
+      <c r="G52" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F53" s="4">
+        <v>200</v>
+      </c>
+      <c r="G53" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F54" s="4">
+        <v>200</v>
+      </c>
+      <c r="G54" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F55" s="4">
+        <v>200</v>
+      </c>
+      <c r="G55" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F56" s="4">
+        <v>200</v>
+      </c>
+      <c r="G56" s="4">
+        <v>100000</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:G14"/>
@@ -23029,7 +24767,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -24763,7 +26501,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -28098,11 +29836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A66780-5999-4CB7-B600-95BB7A39B0F9}">
-  <dimension ref="A1:J56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A22A5-24BA-4DA0-AF00-982051E7F4CE}">
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -28111,16 +29849,15 @@
     <col min="2" max="2" width="24.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -28148,11 +29885,8 @@
       <c r="I1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1274</v>
       </c>
@@ -28166,7 +29900,7 @@
         <v>1276</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F2" s="4">
         <v>200</v>
@@ -28180,9 +29914,8 @@
       <c r="I2" s="4" t="s">
         <v>1277</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1278</v>
       </c>
@@ -28196,7 +29929,7 @@
         <v>1279</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F3" s="4">
         <v>200</v>
@@ -28210,9 +29943,8 @@
       <c r="I3" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1281</v>
       </c>
@@ -28226,7 +29958,7 @@
         <v>1282</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F4" s="4">
         <v>200</v>
@@ -28240,9 +29972,8 @@
       <c r="I4" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>1284</v>
       </c>
@@ -28256,7 +29987,7 @@
         <v>1285</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F5" s="4">
         <v>200</v>
@@ -28270,9 +30001,8 @@
       <c r="I5" s="4" t="s">
         <v>1286</v>
       </c>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>1287</v>
       </c>
@@ -28286,7 +30016,7 @@
         <v>1288</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F6" s="4">
         <v>200</v>
@@ -28300,9 +30030,8 @@
       <c r="I6" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>1289</v>
       </c>
@@ -28316,7 +30045,7 @@
         <v>1290</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F7" s="4">
         <v>200</v>
@@ -28330,9 +30059,8 @@
       <c r="I7" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1291</v>
       </c>
@@ -28346,7 +30074,7 @@
         <v>1292</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F8" s="4">
         <v>200</v>
@@ -28360,9 +30088,8 @@
       <c r="I8" s="4" t="s">
         <v>1293</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>1294</v>
       </c>
@@ -28376,7 +30103,7 @@
         <v>1295</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F9" s="4">
         <v>200</v>
@@ -28390,9 +30117,8 @@
       <c r="I9" s="4" t="s">
         <v>1296</v>
       </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>1297</v>
       </c>
@@ -28406,7 +30132,7 @@
         <v>1298</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F10" s="4">
         <v>200</v>
@@ -28420,9 +30146,8 @@
       <c r="I10" s="4" t="s">
         <v>1299</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>1300</v>
       </c>
@@ -28436,7 +30161,7 @@
         <v>1301</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F11" s="4">
         <v>200</v>
@@ -28450,9 +30175,8 @@
       <c r="I11" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>1302</v>
       </c>
@@ -28466,7 +30190,7 @@
         <v>1303</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F12" s="4">
         <v>200</v>
@@ -28480,9 +30204,8 @@
       <c r="I12" s="4" t="s">
         <v>1304</v>
       </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>1305</v>
       </c>
@@ -28496,7 +30219,7 @@
         <v>1306</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F13" s="4">
         <v>200</v>
@@ -28510,9 +30233,8 @@
       <c r="I13" s="4" t="s">
         <v>1307</v>
       </c>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>1308</v>
       </c>
@@ -28526,7 +30248,7 @@
         <v>1309</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F14" s="4">
         <v>200</v>
@@ -28540,9 +30262,8 @@
       <c r="I14" s="4" t="s">
         <v>1277</v>
       </c>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>1310</v>
       </c>
@@ -28554,7 +30275,7 @@
         <v>1311</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F15" s="4">
         <v>200</v>
@@ -28568,11 +30289,8 @@
       <c r="I15" s="4" t="s">
         <v>1312</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>1313</v>
       </c>
@@ -28584,7 +30302,7 @@
         <v>1275</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F16" s="4">
         <v>200</v>
@@ -28598,11 +30316,8 @@
       <c r="I16" s="4" t="s">
         <v>1314</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>1315</v>
       </c>
@@ -28614,7 +30329,7 @@
         <v>1316</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F17" s="4">
         <v>200</v>
@@ -28626,9 +30341,8 @@
         <v>510</v>
       </c>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>1317</v>
       </c>
@@ -28640,7 +30354,7 @@
         <v>1318</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F18" s="4">
         <v>200</v>
@@ -28652,9 +30366,8 @@
         <v>76</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>1319</v>
       </c>
@@ -28666,7 +30379,7 @@
         <v>1320</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F19" s="4">
         <v>200</v>
@@ -28678,9 +30391,8 @@
         <v>76</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>1321</v>
       </c>
@@ -28692,7 +30404,7 @@
         <v>1322</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F20" s="7">
         <v>200</v>
@@ -28704,9 +30416,8 @@
         <v>510</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>1323</v>
       </c>
@@ -28718,7 +30429,7 @@
         <v>1324</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F21" s="4">
         <v>200</v>
@@ -28730,9 +30441,8 @@
         <v>76</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>1325</v>
       </c>
@@ -28746,7 +30456,7 @@
         <v>1326</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F22" s="4">
         <v>200</v>
@@ -28760,11 +30470,8 @@
       <c r="I22" s="4" t="s">
         <v>1327</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>1328</v>
       </c>
@@ -28778,7 +30485,7 @@
         <v>1329</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F23" s="4">
         <v>200</v>
@@ -28792,11 +30499,8 @@
       <c r="I23" s="4" t="s">
         <v>1330</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>1331</v>
       </c>
@@ -28810,7 +30514,7 @@
         <v>1332</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F24" s="4">
         <v>200</v>
@@ -28822,9 +30526,8 @@
         <v>80</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>1333</v>
       </c>
@@ -28838,7 +30541,7 @@
         <v>1334</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F25" s="4">
         <v>200</v>
@@ -28850,9 +30553,8 @@
         <v>76</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>1335</v>
       </c>
@@ -28866,7 +30568,7 @@
         <v>1336</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F26" s="4">
         <v>200</v>
@@ -28878,9 +30580,8 @@
         <v>76</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>1337</v>
       </c>
@@ -28894,7 +30595,7 @@
         <v>1338</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F27" s="7">
         <v>200</v>
@@ -28906,9 +30607,8 @@
         <v>510</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>1339</v>
       </c>
@@ -28922,7 +30622,7 @@
         <v>1340</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F28" s="4">
         <v>200</v>
@@ -28934,9 +30634,8 @@
         <v>76</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>1341</v>
       </c>
@@ -28950,7 +30649,7 @@
         <v>1342</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F29" s="4">
         <v>200</v>
@@ -28964,9 +30663,8 @@
       <c r="I29" s="4" t="s">
         <v>1327</v>
       </c>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>1343</v>
       </c>
@@ -28980,7 +30678,7 @@
         <v>1344</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F30" s="4">
         <v>200</v>
@@ -28994,11 +30692,8 @@
       <c r="I30" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J30" s="4" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>1346</v>
       </c>
@@ -29012,7 +30707,7 @@
         <v>1347</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F31" s="4">
         <v>200</v>
@@ -29026,11 +30721,8 @@
       <c r="I31" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J31" s="4" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>1348</v>
       </c>
@@ -29044,7 +30736,7 @@
         <v>1349</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F32" s="4">
         <v>200</v>
@@ -29058,11 +30750,8 @@
       <c r="I32" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J32" s="4" t="s">
-        <v>1407</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>1350</v>
       </c>
@@ -29076,7 +30765,7 @@
         <v>1351</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F33" s="4">
         <v>200</v>
@@ -29090,11 +30779,8 @@
       <c r="I33" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>1352</v>
       </c>
@@ -29108,7 +30794,7 @@
         <v>1353</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F34" s="4">
         <v>200</v>
@@ -29122,11 +30808,8 @@
       <c r="I34" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>1409</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>1354</v>
       </c>
@@ -29140,7 +30823,7 @@
         <v>1355</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F35" s="4">
         <v>200</v>
@@ -29154,11 +30837,8 @@
       <c r="I35" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>1356</v>
       </c>
@@ -29172,7 +30852,7 @@
         <v>1357</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F36" s="4">
         <v>200</v>
@@ -29186,11 +30866,8 @@
       <c r="I36" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>1358</v>
       </c>
@@ -29204,7 +30881,7 @@
         <v>1359</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F37" s="4">
         <v>200</v>
@@ -29218,11 +30895,8 @@
       <c r="I37" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J37" s="4" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>1360</v>
       </c>
@@ -29236,7 +30910,7 @@
         <v>1361</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F38" s="4">
         <v>200</v>
@@ -29250,11 +30924,8 @@
       <c r="I38" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J38" s="4" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>1362</v>
       </c>
@@ -29268,7 +30939,7 @@
         <v>1363</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F39" s="4">
         <v>200</v>
@@ -29282,11 +30953,8 @@
       <c r="I39" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J39" s="4" t="s">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>1364</v>
       </c>
@@ -29300,7 +30968,7 @@
         <v>1365</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F40" s="4">
         <v>200</v>
@@ -29314,11 +30982,8 @@
       <c r="I40" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J40" s="4" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>1366</v>
       </c>
@@ -29332,7 +30997,7 @@
         <v>1367</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F41" s="4">
         <v>200</v>
@@ -29346,11 +31011,8 @@
       <c r="I41" s="4" t="s">
         <v>1345</v>
       </c>
-      <c r="J41" s="4" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>1368</v>
       </c>
@@ -29364,7 +31026,7 @@
         <v>1369</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F42" s="4">
         <v>200</v>
@@ -29378,11 +31040,8 @@
       <c r="I42" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="J42" s="4" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>1371</v>
       </c>
@@ -29396,7 +31055,7 @@
         <v>1372</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F43" s="4">
         <v>200</v>
@@ -29410,11 +31069,8 @@
       <c r="I43" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="J43" s="4" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>1373</v>
       </c>
@@ -29426,7 +31082,7 @@
         <v>1374</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F44" s="4">
         <v>200</v>
@@ -29440,9 +31096,8 @@
       <c r="I44" s="4" t="s">
         <v>1370</v>
       </c>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>1375</v>
       </c>
@@ -29456,7 +31111,7 @@
         <v>1376</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F45" s="4">
         <v>200</v>
@@ -29470,11 +31125,8 @@
       <c r="I45" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J45" s="4" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>1378</v>
       </c>
@@ -29488,7 +31140,7 @@
         <v>1379</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F46" s="4">
         <v>200</v>
@@ -29502,11 +31154,8 @@
       <c r="I46" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J46" s="4" t="s">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>1380</v>
       </c>
@@ -29520,7 +31169,7 @@
         <v>1381</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F47" s="4">
         <v>200</v>
@@ -29534,11 +31183,8 @@
       <c r="I47" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J47" s="4" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>1382</v>
       </c>
@@ -29552,7 +31198,7 @@
         <v>1383</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F48" s="4">
         <v>200</v>
@@ -29566,11 +31212,8 @@
       <c r="I48" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J48" s="4" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>1384</v>
       </c>
@@ -29584,7 +31227,7 @@
         <v>1385</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F49" s="4">
         <v>200</v>
@@ -29598,11 +31241,8 @@
       <c r="I49" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J49" s="4" t="s">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>1386</v>
       </c>
@@ -29616,7 +31256,7 @@
         <v>1387</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F50" s="4">
         <v>200</v>
@@ -29630,11 +31270,8 @@
       <c r="I50" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>1388</v>
       </c>
@@ -29648,7 +31285,7 @@
         <v>1389</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F51" s="4">
         <v>200</v>
@@ -29662,11 +31299,8 @@
       <c r="I51" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J51" s="4" t="s">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>1390</v>
       </c>
@@ -29680,7 +31314,7 @@
         <v>1391</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F52" s="4">
         <v>200</v>
@@ -29694,11 +31328,8 @@
       <c r="I52" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J52" s="4" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>1392</v>
       </c>
@@ -29712,7 +31343,7 @@
         <v>1393</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F53" s="4">
         <v>200</v>
@@ -29726,11 +31357,8 @@
       <c r="I53" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J53" s="4" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>1394</v>
       </c>
@@ -29744,7 +31372,7 @@
         <v>1395</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F54" s="4">
         <v>200</v>
@@ -29758,11 +31386,8 @@
       <c r="I54" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>1423</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>1396</v>
       </c>
@@ -29776,7 +31401,7 @@
         <v>1397</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F55" s="4">
         <v>200</v>
@@ -29790,11 +31415,8 @@
       <c r="I55" s="4" t="s">
         <v>1377</v>
       </c>
-      <c r="J55" s="4" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:9" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>1398</v>
       </c>
@@ -29808,7 +31430,7 @@
         <v>1399</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>1400</v>
+        <v>1574</v>
       </c>
       <c r="F56" s="4">
         <v>200</v>
@@ -29821,9 +31443,6 @@
       </c>
       <c r="I56" s="4" t="s">
         <v>1377</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>601</v>
       </c>
     </row>
   </sheetData>
@@ -29835,7 +31454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E763127F-428B-4E62-A7DD-499DA6085963}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update test cases for restful enhance
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2096CF-CA9A-48DC-9451-CEE98219F488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384A5F38-16AC-420A-A18A-2A4D3A22D58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -17036,7 +17036,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -22297,8 +22297,8 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -24416,8 +24416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -29839,7 +29839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971A22A5-24BA-4DA0-AF00-982051E7F4CE}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -31455,7 +31455,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add tests for supporting SQL query capability in Data Layer
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D6F238-0487-4985-8DA9-5843E0BAFF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D14732-CDBB-40F9-BAE6-AAD80A0C776E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="testWhichVerifyRspdata" sheetId="19" r:id="rId13"/>
     <sheet name="testMultiDataSource" sheetId="20" r:id="rId14"/>
     <sheet name="readWriteSqlServer-bc" sheetId="23" r:id="rId15"/>
+    <sheet name="sendSqlToDatalayerVerifyResults" sheetId="26" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="1665">
   <si>
     <t>description</t>
   </si>
@@ -16648,6 +16649,276 @@
       "reserved_field_2": null
     }
 }</t>
+  </si>
+  <si>
+    <t>sqlToDatalayer</t>
+  </si>
+  <si>
+    <t>sqlToOracle</t>
+  </si>
+  <si>
+    <t>SELECT MAX(id) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT count( * ) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT count(department) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(DISTINCT department) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT MIN(id) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT SUM(id) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department LIKE '%BOSS%' AND "POSITION" = 'CEO'</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department LIKE '%BOSS%' OR "POSITION" = 'IM'</t>
+  </si>
+  <si>
+    <t>SELECT TRIM(DEPARTMENT) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT TRIM(ID) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE id between 5 and 10</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE DEPARTMENT between 'BUSINESS_DEPT_1' and 'BUSINESS_DEPT_5'</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DEPT', 'NEW_NAME') new_department FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DEPT', 'NEW_NAME') new_department FROM JINZUDEV.TB_SYS_USER WHERE id = 1</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DE', 'NEW_NAME_') new_department FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT department , SUBSTR(department,2,6) new_department FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE SUBSTR(department,2,6) in ('OSS_DE', 'SSET_D')</t>
+  </si>
+  <si>
+    <t>SELECT username, department , CONCAT(username, department) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT LOWER(department) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t>SELECT UPPER(department) FROM JINZUDEV.TB_SYS_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT abs(parent_id) FROM datalayer.datalayer.Dept </t>
+  </si>
+  <si>
+    <t>SELECT abs(parent_id) FROM JINZUDEV.TB_SYS_DEPT</t>
+  </si>
+  <si>
+    <t>SELECT id, issue_time, event, lease_id FROM datalayer.datalayer.Alarm</t>
+  </si>
+  <si>
+    <t>SELECT id, ccid, latitude, longitude FROM datalayer.datalayer.IotRealtimeData</t>
+  </si>
+  <si>
+    <t>SELECT id, ccid, latitude, longitude FROM JINZUDEV.IOT_REALTIME_DATA</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,NEW_COLUMN mn,employee_number,"POSITION" ,department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department LIKE '%DEPT_3'</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department LIKE 'MANAGEMENT%'</t>
+  </si>
+  <si>
+    <t>SELECT AVG(id), department FROM JINZUDEV.TB_SYS_USER GROUP BY department order by department</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(id), department FROM JINZUDEV.TB_SYS_USER GROUP BY department order by department</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(id), department FROM JINZUDEV.TB_SYS_USER GROUP BY department HAVING department LIKE '%BUSINESS%' order by department</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT department FROM JINZUDEV.TB_SYS_USER order by department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM JINZUDEV.TB_SYS_USER u LEFT JOIN JINZUDEV.TB_SYS_USER_ROLE ur ON u.id = ur.user_id LEFT JOIN JINZUDEV.TB_SYS_ROLE r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM JINZUDEV.TB_SYS_USER u RIGHT JOIN JINZUDEV.TB_SYS_USER_ROLE ur ON u.id = ur.user_id RIGHT JOIN JINZUDEV.TB_SYS_ROLE r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM JINZUDEV.TB_SYS_USER u INNER JOIN JINZUDEV.TB_SYS_USER_ROLE ur ON u.id = ur.user_id INNER JOIN JINZUDEV.TB_SYS_ROLE r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM JINZUDEV.TB_SYS_USER u, JINZUDEV.TB_SYS_USER_ROLE ur, JINZUDEV.TB_SYS_ROLE r WHERE u.id = ur.user_id AND r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE id IN (1,2,3) ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department IN (SELECT dept_key FROM JINZUDEV.TB_SYS_DEPT WHERE id = 1)</t>
+  </si>
+  <si>
+    <t>SELECT department FROM JINZUDEV.TB_SYS_USER INTERSECT SELECT dept_key FROM JINZUDEV.TB_SYS_DEPT ORDER BY department</t>
+  </si>
+  <si>
+    <t>SELECT id, remarks, sort, parent_id, dept_name, dept_key FROM datalayer.datalayer.Dept ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT id, remarks, sort, parent_id, dept_name, dept_key FROM JINZUDEV.TB_SYS_DEPT ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT a_id, issue_time, event, lease_id FROM JINZUDEV.ALARM</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE department LIKE '%OSS_DE%' ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE DEPARTMENT IN ('BOSS_DEPT','ASSET_DEPT','MANAGEMENT_DEPT') ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE rownum &lt; 6 ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT DEPARTMENT FROM JINZUDEV.TB_SYS_USER UNION SELECT DEPT_KEY FROM JINZUDEV.TB_SYS_DEPT ORDER BY department</t>
+  </si>
+  <si>
+    <t>SELECT DEPARTMENT FROM JINZUDEV.TB_SYS_USER UNION ALL SELECT DEPT_KEY FROM JINZUDEV.TB_SYS_DEPT ORDER BY department</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE rownum &lt; 9 MINUS SELECT password,deleted,new_column,employee_number,"POSITION",department,remarks,username,id FROM JINZUDEV.TB_SYS_USER WHERE rownum &lt; 4 ORDER BY id</t>
+  </si>
+  <si>
+    <t>autoVerified</t>
+  </si>
+  <si>
+    <t>AVG has bug SDL-10273</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department LIKE '%OSS_DE%' ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department LIKE '%DEPT_3'</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department LIKE 'MANAGEMENT%'</t>
+  </si>
+  <si>
+    <t>SELECT count( * ) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT count(department) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT AVG(id), department FROM datalayer.datalayer."User1" GROUP BY department order by department</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(id), department FROM datalayer.datalayer."User1" GROUP BY department order by department</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(id), department FROM datalayer.datalayer."User1" GROUP BY department HAVING department LIKE '%BUSINESS%' order by department</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(DISTINCT department) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT department FROM datalayer.datalayer."User1" order by department</t>
+  </si>
+  <si>
+    <t>SELECT MAX(id) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT MIN(id) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT SUM(id) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM datalayer.datalayer."User1" u LEFT JOIN datalayer.datalayer.UserRole ur ON u.id = ur.user_id LEFT JOIN datalayer.datalayer."Role" r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM datalayer.datalayer."User1" u RIGHT JOIN datalayer.datalayer.UserRole ur ON u.id = ur.user_id RIGHT JOIN datalayer.datalayer."Role" r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM datalayer.datalayer."User1" u INNER JOIN datalayer.datalayer.UserRole ur ON u.id = ur.user_id INNER JOIN datalayer.datalayer."Role" r ON r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT u.id, u.username, r.role_name FROM datalayer.datalayer."User1" u, datalayer.datalayer.UserRole ur, datalayer.datalayer."Role" r WHERE u.id = ur.user_id AND r.id = ur.role_id ORDER BY u.id, u.username, r.role_name DESC </t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department LIKE '%BOSS%' AND "position" = 'CEO'</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department LIKE '%BOSS%' OR "position" = 'IM'</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE id IN (1,2,3) ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department IN ('BOSS_DEPT','ASSET_DEPT','MANAGEMENT_DEPT') ORDER BY id</t>
+  </si>
+  <si>
+    <t>SELECT department FROM datalayer.datalayer."User1" UNION SELECT dept_key FROM datalayer.datalayer.Dept ORDER BY department</t>
+  </si>
+  <si>
+    <t>SELECT department FROM datalayer.datalayer."User1" UNION ALL SELECT dept_key FROM datalayer.datalayer.Dept ORDER BY department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" ORDER BY id limit 5 </t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" ORDER BY id limit 5 offset 3</t>
+  </si>
+  <si>
+    <t>SELECT TRIM(department) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT TRIM(id) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE id between 5 and 10</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE DEPARTMENT between 'BUSINESS_DEPT_1' and 'BUSINESS_DEPT_5'</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DEPT', 'NEW_NAME') new_department FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DEPT', 'NEW_NAME') new_department FROM datalayer.datalayer."User1" WHERE id = 1</t>
+  </si>
+  <si>
+    <t>SELECT department , REPLACE(department, 'DE', 'NEW_NAME_') new_department FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT department , SUBSTRING(department,2,6) new_department FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE SUBSTRING(department,2,6) in ('OSS_DE', 'SSET_D')</t>
+  </si>
+  <si>
+    <t>SELECT username, department , CONCAT(username, department) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT password,deleted,new_colomn,employee_number,"position",department,remarks,username,id FROM datalayer.datalayer."User1" WHERE department IN (SELECT dept_key FROM datalayer.datalayer.Dept WHERE id = 1)</t>
+  </si>
+  <si>
+    <t>SELECT department FROM datalayer.datalayer."User1" INTERSECT SELECT dept_key FROM datalayer.datalayer.Dept ORDER BY department</t>
+  </si>
+  <si>
+    <t>SELECT LOWER(department) FROM datalayer.datalayer."User1"</t>
+  </si>
+  <si>
+    <t>SELECT UPPER(department) FROM datalayer.datalayer."User1"</t>
   </si>
 </sst>
 </file>
@@ -18559,7 +18830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD7D6DE-617D-4A49-9D87-297640E0E1DC}">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+    <sheetView topLeftCell="A102" workbookViewId="0">
       <selection activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
@@ -24405,6 +24676,528 @@
       </c>
       <c r="J56" s="4" t="s">
         <v>601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078B81E0-CD90-42CA-9CB8-525B3F9B88C1}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="85.77734375" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1624</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1649</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1657</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test cases for iot-demo-test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858239C9-E3BD-49A1-96F0-260D65667848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A9667-DAA1-4705-9388-0F0920A3B2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16842,7 +16842,7 @@
       "json_value": [
         {
           "code": 1,
-          "data": "Conditions parse error(syntax error or field not exist in mapper) (\"id\" not in ('1', '2', '3'))"
+          "data": "Conditions parse error(syntax error or field not exist in mapper) (id not in ('1', '2', '3'))"
         }
       ],
       "reserved_field_1": null,
@@ -16856,7 +16856,7 @@
       "json_value": [
         {
           "code": 1,
-          "data": "Conditions parse error(syntax error or field not exist in mapper) (\"id\" = '1' and \"id\" in ('2', '3'))"
+          "data": "Conditions parse error(syntax error or field not exist in mapper) (id = '1' and id in ('2', '3'))"
         }
       ],
       "reserved_field_1": null,
@@ -16870,7 +16870,7 @@
       "json_value": [
         {
           "code": 1,
-          "data": "Conditions parse error(syntax error or field not exist in mapper) (\"id\" = '1' and \"name\" = 'name1' and \"age\" = '11' and(\"id\", \"name\", \"age\") in (('5', 'name5', '15'),('6', 'name6', '16')))"
+          "data": "Conditions parse error(syntax error or field not exist in mapper) (id = '1' and name = 'name1' and age = '11' and(id, name, age) in (('5', 'name5', '15'),('6', 'name6', '16')))"
         }
       ],
       "reserved_field_1": null,
@@ -16884,7 +16884,7 @@
       "json_value": [
         {
           "code": 1,
-          "data": "Conditions parse error(syntax error or field not exist in mapper) (\"id\" = '1' and \"name\" = 'name1' and \"age\" = '11' and(\"id\", \"name\", \"age\") in (('5', 'name5', '15'),('6', 'name6', '16')))"
+          "data": "Conditions parse error(syntax error or field not exist in mapper) (id = '1' and name = 'name1' and age = '11' and(id, name, age) in (('5', 'name5', '15'),('6', 'name6', '16')))"
         }
       ],
       "reserved_field_1": null,
@@ -16898,7 +16898,7 @@
       "json_value": [
         {
           "code": 1,
-          "data": "Conditions parse error(syntax error or field not exist in mapper) (\"id\" = '1' and \"name\" = 'name1' and \"age\" = '11' and(\"id\", \"name\", \"age\") in (('5', 'name5', '15'),('6', 'name6', '16')))"
+          "data": "Conditions parse error(syntax error or field not exist in mapper) (id = '1' and name = 'name1' and age = '11' and(id, name, age) in (('5', 'name5', '15'),('6', 'name6', '16')))"
         }
       ],
       "reserved_field_1": null,

</xml_diff>

<commit_message>
update test case for iot
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5084A031-CEFA-45D3-8538-F32F73E6EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50798B42-D192-47A1-B8F3-8D3F304CBBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="743" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -16654,9 +16654,6 @@
     <t>SELECT UPPER(department) FROM datalayer.datalayer."User1"</t>
   </si>
   <si>
-    <t>{SINAMICS_300_Log(cond:"{Abs_actual_current_smoothed: {_gt: 19.999}}")  {update_time}}</t>
-  </si>
-  <si>
     <t>{SINAMICS_300_Log {update_time}}</t>
   </si>
   <si>
@@ -16905,6 +16902,9 @@
         }
     }
 ]</t>
+  </si>
+  <si>
+    <t>{SINAMICS_300_Log(cond:"{Abs_actual_current_smoothed: {_gt: 199.999}}")  {update_time}}</t>
   </si>
 </sst>
 </file>
@@ -18225,7 +18225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD7C303-AF77-4B95-95EB-BAA32E85C8DA}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -18288,7 +18288,7 @@
         <v>209</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>211</v>
@@ -18323,7 +18323,7 @@
         <v>216</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>211</v>
@@ -18358,7 +18358,7 @@
         <v>217</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>211</v>
@@ -18393,7 +18393,7 @@
         <v>218</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>211</v>
@@ -18428,7 +18428,7 @@
         <v>219</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>211</v>
@@ -18463,7 +18463,7 @@
         <v>231</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>232</v>
@@ -18498,7 +18498,7 @@
         <v>237</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>232</v>
@@ -18533,7 +18533,7 @@
         <v>238</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>232</v>
@@ -18568,7 +18568,7 @@
         <v>239</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>232</v>
@@ -18603,7 +18603,7 @@
         <v>240</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>232</v>
@@ -18638,7 +18638,7 @@
         <v>242</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>243</v>
@@ -18673,7 +18673,7 @@
         <v>237</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>243</v>
@@ -18708,7 +18708,7 @@
         <v>900</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>243</v>
@@ -18743,7 +18743,7 @@
         <v>901</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>243</v>
@@ -18778,7 +18778,7 @@
         <v>902</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>243</v>
@@ -21464,7 +21464,7 @@
         <v>10</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -21644,7 +21644,7 @@
         <v>10</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -21902,7 +21902,7 @@
         <v>10</v>
       </c>
       <c r="H120" s="4" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -22134,7 +22134,7 @@
         <v>10</v>
       </c>
       <c r="H129" s="4" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -22366,7 +22366,7 @@
         <v>10</v>
       </c>
       <c r="H138" s="4" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -22727,7 +22727,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -25195,8 +25195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -25495,7 +25495,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>1649</v>
+        <v>1661</v>
       </c>
       <c r="D13" s="4">
         <v>200</v>
@@ -25518,7 +25518,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D14" s="4">
         <v>200</v>

</xml_diff>